<commit_message>
Documentos de HU y MVH
</commit_message>
<xml_diff>
--- a/DESARROLLO/SAV/GESTION/SAV-MVH.xlsx
+++ b/DESARROLLO/SAV/GESTION/SAV-MVH.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A1FC69-C029-4D93-A83E-657B87C38C78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>TAREAS</t>
   </si>
@@ -83,12 +84,66 @@
   </si>
   <si>
     <t>RELEASE 2</t>
+  </si>
+  <si>
+    <t>AULAS</t>
+  </si>
+  <si>
+    <t>REPORTES</t>
+  </si>
+  <si>
+    <t>H17 - Visualizar Aulas</t>
+  </si>
+  <si>
+    <t>H18 - Agregar Aula</t>
+  </si>
+  <si>
+    <t>ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>MATRICULA</t>
+  </si>
+  <si>
+    <t>H19 - Acceder Aula</t>
+  </si>
+  <si>
+    <t>H20 - Editar Aula</t>
+  </si>
+  <si>
+    <t>H21 - Eliminar Aula</t>
+  </si>
+  <si>
+    <t>H22 - Visualizar estudiantes</t>
+  </si>
+  <si>
+    <t>H23 - Agregar estudiante</t>
+  </si>
+  <si>
+    <t>H 24 - Editar estudiante</t>
+  </si>
+  <si>
+    <t>H23 - Visualizar tareas Asignadas</t>
+  </si>
+  <si>
+    <t>H26 - Agregar tareas</t>
+  </si>
+  <si>
+    <t>H28 - Generar examen</t>
+  </si>
+  <si>
+    <t>H29 - Visualizar reporte de alumnos</t>
+  </si>
+  <si>
+    <t>H27 - Matricular estudiantes</t>
+  </si>
+  <si>
+    <t>RELEASE 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -148,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -169,6 +224,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -264,6 +325,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -299,6 +377,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,11 +569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -488,11 +583,14 @@
     <col min="3" max="3" width="17.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="17" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="18.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="16" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -508,15 +606,32 @@
       <c r="E1" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="9" customHeight="1">
+      <c r="F1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="9" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="39.6">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="39.6">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -524,7 +639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.4">
+    <row r="4" spans="1:10" ht="26.4">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -533,7 +648,7 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="39.6">
+    <row r="5" spans="1:10" ht="39.6">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -544,24 +659,32 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="39.6">
+    <row r="6" spans="1:10" ht="39.6">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="9" customHeight="1">
+    <row r="7" spans="1:10" ht="9" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="39.6">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="39.6">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
@@ -578,8 +701,11 @@
         <v>10</v>
       </c>
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="39.6">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="39.6">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -592,54 +718,114 @@
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="9" customHeight="1">
+    <row r="10" spans="1:10" ht="9" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" ht="39.6" customHeight="1">
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1">
-      <c r="A12" s="4"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="39.6" customHeight="1">
+      <c r="A11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="10"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" ht="28.8">
+      <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.4" customHeight="1">
-      <c r="A15" s="4"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="14.4" customHeight="1">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.4" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>